<commit_message>
started adding atf trawl
</commit_message>
<xml_diff>
--- a/Data/data-raw/GOA/Pollock 2018/Rceattle_pollock_2018.xlsx
+++ b/Data/data-raw/GOA/Pollock 2018/Rceattle_pollock_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/RceattleRuns/Data/data-raw/GOA/Pollock 2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D505924-42CA-644F-98ED-DF539983D1E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5311F5EA-D4DC-B34C-92E0-020515673112}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13920" activeTab="4" xr2:uid="{075EC1A9-A118-934F-9672-DCD5B7DE9E6F}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13920" activeTab="7" xr2:uid="{075EC1A9-A118-934F-9672-DCD5B7DE9E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="control" sheetId="8" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="srv_biom" sheetId="5" r:id="rId6"/>
     <sheet name="srv_comp" sheetId="6" r:id="rId7"/>
     <sheet name="wt" sheetId="7" r:id="rId8"/>
+    <sheet name="age_error" sheetId="9" r:id="rId9"/>
+    <sheet name="alk" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -749,6 +751,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0FE08A-9F4D-7B40-805C-2BB0424F64DC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3B8E63-BAA6-3747-B823-8A3721B46933}">
   <dimension ref="A1:I2"/>
@@ -4312,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49ACC92-2BAC-754A-8430-EFA2D58A0CDA}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -9170,8 +9184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917D4A9B-970E-C542-9F8F-DF18BFDE4724}">
   <dimension ref="A1:Y246"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="D204" sqref="D204"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20530,4 +20544,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B25C60F-7F84-6C48-8447-43A4AE21E2B1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>